<commit_message>
Correction de bugs de textures, ajout du paysage de forêt, modification des tempos lors de la cinématique
</commit_message>
<xml_diff>
--- a/Assets/Other/TableauExcel.xlsx
+++ b/Assets/Other/TableauExcel.xlsx
@@ -137,7 +137,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +166,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
@@ -469,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +484,7 @@
     <col min="5" max="5" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
@@ -501,7 +502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -523,7 +524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,319 +537,291 @@
         <v>1.3530092592592594E-2</v>
       </c>
       <c r="D3" s="6">
-        <f>E3-C3</f>
-        <v>2.6851851851851863E-3</v>
+        <v>2.8009259259259259E-3</v>
       </c>
       <c r="E3" s="8">
-        <v>1.621527777777778E-2</v>
+        <f t="shared" ref="E3:E28" si="0">C3+D3</f>
+        <v>1.6331018518518519E-2</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B16" si="0">B3+1</f>
+        <f t="shared" ref="B4:B16" si="1">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="7">
         <f>E3</f>
-        <v>1.621527777777778E-2</v>
+        <v>1.6331018518518519E-2</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" ref="D4:D28" si="1">E4-C4</f>
-        <v>2.5810185185185172E-3</v>
+        <v>2.5810185185185185E-3</v>
       </c>
       <c r="E4" s="8">
-        <v>1.8796296296296297E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.8912037037037036E-2</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C5" s="7">
         <f>E4</f>
-        <v>1.8796296296296297E-2</v>
+        <v>1.8912037037037036E-2</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" si="1"/>
-        <v>5.0462962962962987E-3</v>
+        <v>5.0578703703703706E-3</v>
       </c>
       <c r="E5" s="8">
-        <v>2.3842592592592596E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.3969907407407405E-2</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C6" s="7">
         <f t="shared" ref="C6:C25" si="2">E5</f>
-        <v>2.3842592592592596E-2</v>
+        <v>2.3969907407407405E-2</v>
       </c>
       <c r="D6" s="6">
-        <f t="shared" si="1"/>
-        <v>2.4305555555555573E-3</v>
+        <v>5.3622685185185183E-2</v>
       </c>
       <c r="E6" s="8">
-        <v>2.6273148148148153E-2</v>
+        <f>C6+D6</f>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="2"/>
-        <v>2.6273148148148153E-2</v>
-      </c>
-      <c r="D7" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3">
         <f t="shared" si="1"/>
-        <v>5.4976851851851846E-2</v>
-      </c>
-      <c r="E7" s="8">
-        <v>8.1250000000000003E-2</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C8" s="7">
         <f t="shared" si="2"/>
-        <v>8.1250000000000003E-2</v>
-      </c>
-      <c r="D8" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
         <f t="shared" si="1"/>
-        <v>-8.1250000000000003E-2</v>
-      </c>
-      <c r="E8" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="3">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C12" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C13" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C14" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C15" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C16" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D16" s="6"/>
       <c r="E16" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>7</v>
@@ -864,15 +837,12 @@
       </c>
       <c r="C17" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D17" s="6"/>
       <c r="E17" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>7</v>
@@ -888,15 +858,12 @@
       </c>
       <c r="C18" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D18" s="6"/>
       <c r="E18" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>7</v>
@@ -912,15 +879,12 @@
       </c>
       <c r="C19" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D19" s="6"/>
       <c r="E19" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>7</v>
@@ -936,15 +900,12 @@
       </c>
       <c r="C20" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D20" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D20" s="6"/>
       <c r="E20" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>7</v>
@@ -960,15 +921,12 @@
       </c>
       <c r="C21" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D21" s="6"/>
       <c r="E21" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>7</v>
@@ -984,15 +942,12 @@
       </c>
       <c r="C22" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D22" s="6"/>
       <c r="E22" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>7</v>
@@ -1008,15 +963,12 @@
       </c>
       <c r="C23" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>7</v>
@@ -1032,15 +984,12 @@
       </c>
       <c r="C24" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D24" s="6"/>
       <c r="E24" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>7</v>
@@ -1056,15 +1005,12 @@
       </c>
       <c r="C25" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D25" s="6"/>
       <c r="E25" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>7</v>
@@ -1080,15 +1026,12 @@
       </c>
       <c r="C26" s="7">
         <f t="shared" ref="C26:C27" si="5">E25</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D26" s="6"/>
       <c r="E26" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>7</v>
@@ -1104,15 +1047,12 @@
       </c>
       <c r="C27" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D27" s="6"/>
       <c r="E27" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>7</v>
@@ -1128,15 +1068,12 @@
       </c>
       <c r="C28" s="7">
         <f t="shared" ref="C28" si="7">E27</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>7.7592592592592588E-2</v>
+      </c>
+      <c r="D28" s="6"/>
       <c r="E28" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.7592592592592588E-2</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>7</v>
@@ -1151,7 +1088,7 @@
     <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C31" s="5">
         <f>E7</f>
-        <v>8.1250000000000003E-2</v>
+        <v>7.7592592592592588E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>